<commit_message>
adicionando alguns procedimentos no db e tirando acentos dos nomes das colunas ( municipio)
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalves\Downloads\projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\OBSERVATORIO\PROJETOS\BI e Afins\MARQUE FACIL\analise_relatorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBF3CBE-BB77-4165-B44A-63FA2EC435C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B522A6B-7B36-4386-8AB9-8D0A3DEC9BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AI$216</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="d0fWzVjk1oQ2FUQg16CP8B3860lrCnVB2sZf10b2GsA="/>
     </ext>
@@ -28,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="486">
   <si>
     <t>AUDIOMETRIA TONAL LIMIAR IMPED e LOGOAUDOMETRIA (LDV-IRF-LRF)</t>
   </si>
@@ -1477,13 +1488,23 @@
   </si>
   <si>
     <t>RETINOGRAFIA FLUORESCENTE BINOCULAR</t>
+  </si>
+  <si>
+    <t>ULTRASSONOGRAFIA DE ARTICULACAO E PARTES MOLES</t>
+  </si>
+  <si>
+    <t>TOMOGRAFIA COMPUTADORIZADA DE CRANIO</t>
+  </si>
+  <si>
+    <t>CONSULTA - GINECOLOGIA E COLETA MATERIAL EXAME CITOPATOLOGICO
+COLO UTERINO C/ RESULTADO E CONSULTA DE RETORNO GINECOLOGIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1515,6 +1536,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1542,7 +1578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1555,6 +1591,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1772,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2068,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
@@ -2066,7 +2107,9 @@
         <v>58</v>
       </c>
       <c r="R3" s="4"/>
-      <c r="S3" s="3"/>
+      <c r="S3" s="9" t="s">
+        <v>485</v>
+      </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3" t="s">
@@ -2362,7 +2405,7 @@
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="3"/>
+      <c r="S8" s="10"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -2431,7 +2474,7 @@
         <v>101</v>
       </c>
       <c r="AD9" s="3" t="s">
-        <v>102</v>
+        <v>484</v>
       </c>
       <c r="AE9" s="6" t="s">
         <v>103</v>
@@ -2485,8 +2528,8 @@
       <c r="AD10" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AE10" s="6" t="s">
-        <v>109</v>
+      <c r="AE10" s="3" t="s">
+        <v>483</v>
       </c>
       <c r="AF10" s="3" t="s">
         <v>110</v>
@@ -2796,7 +2839,9 @@
       <c r="AB16" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AD16" s="3"/>
+      <c r="AD16" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="AE16" s="6" t="s">
         <v>144</v>
       </c>
@@ -2846,7 +2891,6 @@
       <c r="AB17" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="AD17" s="3"/>
       <c r="AE17" s="6" t="s">
         <v>149</v>
       </c>
@@ -2944,7 +2988,7 @@
       </c>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
-      <c r="AE19" t="s">
+      <c r="AE19" s="8" t="s">
         <v>211</v>
       </c>
       <c r="AF19" s="3"/>
@@ -2990,7 +3034,9 @@
       </c>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
+      <c r="AE20" s="6" t="s">
+        <v>109</v>
+      </c>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
@@ -3034,7 +3080,6 @@
       </c>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
@@ -39751,6 +39796,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>